<commit_message>
Changes to Excel doc
</commit_message>
<xml_diff>
--- a/Labyrinth/Labyrith_doc.xlsx
+++ b/Labyrinth/Labyrith_doc.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edward\Google Drive\Masters\Exercises\Semster1\Intro_to_AI\Project\Labyrith\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edward\Documents\GitHub\AI_Project\Labyrinth\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5145" yWindow="0" windowWidth="28800" windowHeight="13020"/>
+    <workbookView xWindow="6315" yWindow="0" windowWidth="28800" windowHeight="13020"/>
   </bookViews>
   <sheets>
     <sheet name="Pieces" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>Piece</t>
   </si>
@@ -70,6 +70,45 @@
   </si>
   <si>
     <t>0110</t>
+  </si>
+  <si>
+    <t>Representation of maze in java</t>
+  </si>
+  <si>
+    <t>Representation of maze in Prolog (example)</t>
+  </si>
+  <si>
+    <t>[[0110,0101,0111,1100,0111,0011,0011],</t>
+  </si>
+  <si>
+    <t>[1010,0101,1100,1001,0101,1110,0110],</t>
+  </si>
+  <si>
+    <t>[1011,1010,1011,1110,0111,0110,1110],</t>
+  </si>
+  <si>
+    <t>[0101,1001,1100,1101,1001,0111,0101],</t>
+  </si>
+  <si>
+    <t>[1011,1101,1101,0011,1110,1010,1110],</t>
+  </si>
+  <si>
+    <t>[1011,1001,0101,1001,0101,0110,0110],</t>
+  </si>
+  <si>
+    <t>[1100,1010,1101,0101,1101,1001,1001]]</t>
+  </si>
+  <si>
+    <t>Prolog representation</t>
+  </si>
+  <si>
+    <t>0011</t>
+  </si>
+  <si>
+    <t>0101</t>
+  </si>
+  <si>
+    <t>0111</t>
   </si>
 </sst>
 </file>
@@ -93,7 +132,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -106,6 +145,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="30">
     <border>
@@ -486,7 +531,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -547,7 +592,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -558,6 +602,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -573,6 +630,49 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>608692</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>104321</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3139168" y="222250"/>
+          <a:ext cx="3351892" cy="3361871"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -838,10 +938,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:I5"/>
+  <dimension ref="B1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="N32" sqref="N32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -858,6 +958,12 @@
       <c r="D1" t="s">
         <v>13</v>
       </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -869,6 +975,7 @@
       <c r="D2">
         <v>0</v>
       </c>
+      <c r="I2" s="39"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -881,8 +988,9 @@
         <v>1</v>
       </c>
       <c r="F3" s="23"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="25"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="39"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
@@ -894,17 +1002,198 @@
       <c r="D4">
         <v>2</v>
       </c>
-      <c r="F4" s="26"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="32" t="s">
+      <c r="F4" s="25"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="31">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F5" s="28"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="35"/>
+      <c r="I5" s="39"/>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I6" s="39"/>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F7" s="23"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="39"/>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F8" s="37"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="31" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="F5" s="29"/>
-      <c r="G5" s="30"/>
-      <c r="H5" s="31"/>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F9" s="28"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="39"/>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I10" s="39"/>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F11" s="23"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="39"/>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F12" s="33"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="31" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F13" s="28"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="35"/>
+      <c r="I13" s="39"/>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I14" s="39"/>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F15" s="41"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="40"/>
+      <c r="I15" s="39"/>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F16" s="33"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="39">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="17" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F17" s="42"/>
+      <c r="G17" s="34"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="39"/>
+    </row>
+    <row r="18" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="I18" s="39"/>
+    </row>
+    <row r="19" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F19" s="41"/>
+      <c r="G19" s="32"/>
+      <c r="H19" s="40"/>
+    </row>
+    <row r="20" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F20" s="37"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="38"/>
+      <c r="I20">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="21" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F21" s="42"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="35"/>
+    </row>
+    <row r="23" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F23" s="41"/>
+      <c r="G23" s="36"/>
+      <c r="H23" s="40"/>
+    </row>
+    <row r="24" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F24" s="33"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="27"/>
+      <c r="I24" s="31" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F25" s="42"/>
+      <c r="G25" s="34"/>
+      <c r="H25" s="35"/>
+    </row>
+    <row r="27" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F27" s="23"/>
+      <c r="G27" s="32"/>
+      <c r="H27" s="24"/>
+    </row>
+    <row r="28" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F28" s="33"/>
+      <c r="G28" s="26"/>
+      <c r="H28" s="27"/>
+      <c r="I28">
+        <v>1101</v>
+      </c>
+    </row>
+    <row r="29" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F29" s="42"/>
+      <c r="G29" s="34"/>
+      <c r="H29" s="35"/>
+    </row>
+    <row r="31" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F31" s="23"/>
+      <c r="G31" s="32"/>
+      <c r="H31" s="24"/>
+    </row>
+    <row r="32" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F32" s="37"/>
+      <c r="G32" s="26"/>
+      <c r="H32" s="27"/>
+      <c r="I32">
+        <v>1110</v>
+      </c>
+    </row>
+    <row r="33" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F33" s="28"/>
+      <c r="G33" s="29"/>
+      <c r="H33" s="30"/>
+    </row>
+    <row r="35" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F35" s="23"/>
+      <c r="G35" s="36"/>
+      <c r="H35" s="24"/>
+    </row>
+    <row r="36" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F36" s="33"/>
+      <c r="G36" s="26"/>
+      <c r="H36" s="27"/>
+      <c r="I36" s="31" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F37" s="28"/>
+      <c r="G37" s="29"/>
+      <c r="H37" s="35"/>
+    </row>
+    <row r="39" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F39" s="41"/>
+      <c r="G39" s="32"/>
+      <c r="H39" s="40"/>
+    </row>
+    <row r="40" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F40" s="33"/>
+      <c r="G40" s="26"/>
+      <c r="H40" s="27"/>
+      <c r="I40">
+        <v>1101</v>
+      </c>
+    </row>
+    <row r="41" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F41" s="42"/>
+      <c r="G41" s="34"/>
+      <c r="H41" s="35"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -913,315 +1202,346 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J10"/>
+  <dimension ref="B1:Q11"/>
   <sheetViews>
-    <sheetView zoomScale="260" zoomScaleNormal="260" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.625" customWidth="1"/>
-    <col min="2" max="2" width="2.25" customWidth="1"/>
-    <col min="3" max="10" width="2.625" customWidth="1"/>
-    <col min="11" max="11" width="2.5" customWidth="1"/>
+    <col min="2" max="2" width="34.375" customWidth="1"/>
+    <col min="8" max="8" width="8.625" customWidth="1"/>
+    <col min="9" max="9" width="2.25" customWidth="1"/>
+    <col min="10" max="17" width="2.625" customWidth="1"/>
+    <col min="18" max="18" width="2.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="19" t="s">
+    <row r="1" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="20">
+      <c r="K3" s="20">
         <v>0</v>
       </c>
-      <c r="E2" s="20">
+      <c r="L3" s="20">
         <v>1</v>
       </c>
-      <c r="F2" s="20">
+      <c r="M3" s="20">
         <v>2</v>
       </c>
-      <c r="G2" s="20">
+      <c r="N3" s="20">
         <v>3</v>
       </c>
-      <c r="H2" s="20">
+      <c r="O3" s="20">
         <v>4</v>
       </c>
-      <c r="I2" s="20">
+      <c r="P3" s="20">
         <v>5</v>
       </c>
-      <c r="J2" s="21">
+      <c r="Q3" s="21">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="13" t="s">
+    <row r="4" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="16" t="s">
+      <c r="J4" s="22"/>
+      <c r="K4" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="L4" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="M4" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="17" t="s">
+      <c r="N4" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="O4" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="17" t="s">
+      <c r="P4" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="18" t="s">
+      <c r="Q4" s="18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="14">
+    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="14">
         <v>0</v>
       </c>
-      <c r="C4" s="10">
+      <c r="J5" s="10">
         <v>0</v>
       </c>
-      <c r="D4" s="1">
+      <c r="K5" s="1">
         <v>0</v>
       </c>
-      <c r="E4" s="2">
+      <c r="L5" s="2">
         <v>1</v>
       </c>
-      <c r="F4" s="2">
+      <c r="M5" s="2">
         <v>2</v>
       </c>
-      <c r="G4" s="2">
+      <c r="N5" s="2">
         <v>3</v>
       </c>
-      <c r="H4" s="2">
+      <c r="O5" s="2">
         <v>4</v>
       </c>
-      <c r="I4" s="2">
+      <c r="P5" s="2">
         <v>5</v>
       </c>
-      <c r="J4" s="3">
+      <c r="Q5" s="3">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="14">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6" s="14">
         <v>1</v>
       </c>
-      <c r="C5" s="11">
+      <c r="J6" s="11">
         <v>1</v>
       </c>
-      <c r="D5" s="4">
-        <f t="shared" ref="D5:D10" si="0">D4+7</f>
+      <c r="K6" s="4">
+        <f t="shared" ref="K6:K11" si="0">K5+7</f>
         <v>7</v>
       </c>
-      <c r="E5" s="5">
-        <f t="shared" ref="E5:J10" si="1">E4+7</f>
+      <c r="L6" s="5">
+        <f t="shared" ref="L6:Q11" si="1">L5+7</f>
         <v>8</v>
       </c>
-      <c r="F5" s="5">
+      <c r="M6" s="5">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="G5" s="5">
+      <c r="N6" s="5">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="H5" s="5">
+      <c r="O6" s="5">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="I5" s="5">
+      <c r="P6" s="5">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="J5" s="6">
+      <c r="Q6" s="6">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="14">
+    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" s="14">
         <v>2</v>
       </c>
-      <c r="C6" s="11">
+      <c r="J7" s="11">
         <v>2</v>
       </c>
-      <c r="D6" s="4">
+      <c r="K7" s="4">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="E6" s="5">
+      <c r="L7" s="5">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="F6" s="5">
+      <c r="M7" s="5">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="G6" s="5">
+      <c r="N7" s="5">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="H6" s="5">
+      <c r="O7" s="5">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="I6" s="5">
+      <c r="P7" s="5">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="J6" s="6">
+      <c r="Q7" s="6">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="14">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I8" s="14">
         <v>3</v>
       </c>
-      <c r="C7" s="11">
+      <c r="J8" s="11">
         <v>3</v>
       </c>
-      <c r="D7" s="4">
+      <c r="K8" s="4">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="E7" s="5">
+      <c r="L8" s="5">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="F7" s="5">
+      <c r="M8" s="5">
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="G7" s="5">
+      <c r="N8" s="5">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="H7" s="5">
+      <c r="O8" s="5">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="I7" s="5">
+      <c r="P8" s="5">
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="J7" s="6">
+      <c r="Q8" s="6">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="14">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="I9" s="14">
         <v>4</v>
       </c>
-      <c r="C8" s="11">
+      <c r="J9" s="11">
         <v>4</v>
       </c>
-      <c r="D8" s="4">
+      <c r="K9" s="4">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="E8" s="5">
+      <c r="L9" s="5">
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="F8" s="5">
+      <c r="M9" s="5">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="G8" s="5">
+      <c r="N9" s="5">
         <f t="shared" si="1"/>
         <v>31</v>
       </c>
-      <c r="H8" s="5">
+      <c r="O9" s="5">
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="I8" s="5">
+      <c r="P9" s="5">
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="J8" s="6">
+      <c r="Q9" s="6">
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="14">
+    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="I10" s="14">
         <v>5</v>
       </c>
-      <c r="C9" s="11">
+      <c r="J10" s="11">
         <v>5</v>
       </c>
-      <c r="D9" s="4">
+      <c r="K10" s="4">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="E9" s="5">
+      <c r="L10" s="5">
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="F9" s="5">
+      <c r="M10" s="5">
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
-      <c r="G9" s="5">
+      <c r="N10" s="5">
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
-      <c r="H9" s="5">
+      <c r="O10" s="5">
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
-      <c r="I9" s="5">
+      <c r="P10" s="5">
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="J9" s="6">
+      <c r="Q10" s="6">
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="15">
+    <row r="11" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I11" s="15">
         <v>6</v>
       </c>
-      <c r="C10" s="12">
+      <c r="J11" s="12">
         <v>6</v>
       </c>
-      <c r="D10" s="7">
+      <c r="K11" s="7">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="E10" s="8">
+      <c r="L11" s="8">
         <f t="shared" si="1"/>
         <v>43</v>
       </c>
-      <c r="F10" s="8">
+      <c r="M11" s="8">
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
-      <c r="G10" s="8">
+      <c r="N11" s="8">
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
-      <c r="H10" s="8">
+      <c r="O11" s="8">
         <f t="shared" si="1"/>
         <v>46</v>
       </c>
-      <c r="I10" s="8">
+      <c r="P11" s="8">
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
-      <c r="J10" s="9">
+      <c r="Q11" s="9">
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
@@ -1229,5 +1549,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Corrected some incorrectly defined pieces
</commit_message>
<xml_diff>
--- a/Labyrinth/Labyrith_doc.xlsx
+++ b/Labyrinth/Labyrith_doc.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8664" yWindow="0" windowWidth="28800" windowHeight="13020" activeTab="1"/>
+    <workbookView xWindow="9840" yWindow="0" windowWidth="28800" windowHeight="13020"/>
   </bookViews>
   <sheets>
     <sheet name="Pieces" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
   <si>
     <t>Piece</t>
   </si>
@@ -109,6 +109,51 @@
   </si>
   <si>
     <t>0111</t>
+  </si>
+  <si>
+    <t>48,48</t>
+  </si>
+  <si>
+    <t>Treasures</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Ravensburger-26448-Labyrinth/dp/B00000J0JF</t>
+  </si>
+  <si>
+    <t>helmet</t>
+  </si>
+  <si>
+    <t>candle</t>
+  </si>
+  <si>
+    <t>sword</t>
+  </si>
+  <si>
+    <t>opal</t>
+  </si>
+  <si>
+    <t>treasure chest</t>
+  </si>
+  <si>
+    <t>ring</t>
+  </si>
+  <si>
+    <t>skull</t>
+  </si>
+  <si>
+    <t>keys</t>
+  </si>
+  <si>
+    <t>crown</t>
+  </si>
+  <si>
+    <t>map</t>
+  </si>
+  <si>
+    <t>bag of gold</t>
+  </si>
+  <si>
+    <t>book</t>
   </si>
 </sst>
 </file>
@@ -633,6 +678,49 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>148590</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7292340" y="365760"/>
+          <a:ext cx="5514975" cy="4171950"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -938,10 +1026,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:I45"/>
+  <dimension ref="B1:O45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -949,9 +1037,10 @@
     <col min="6" max="6" width="2.88671875" customWidth="1"/>
     <col min="7" max="7" width="2.77734375" customWidth="1"/>
     <col min="8" max="8" width="2.88671875" customWidth="1"/>
+    <col min="12" max="12" width="12.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -964,8 +1053,14 @@
       <c r="I1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="L1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -977,7 +1072,7 @@
       </c>
       <c r="I2" s="39"/>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>2</v>
       </c>
@@ -991,8 +1086,11 @@
       <c r="G3" s="32"/>
       <c r="H3" s="24"/>
       <c r="I3" s="39"/>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="L3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -1008,69 +1106,102 @@
       <c r="I4" s="31">
         <v>1100</v>
       </c>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="L4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
       <c r="F5" s="28"/>
       <c r="G5" s="34"/>
       <c r="H5" s="35"/>
       <c r="I5" s="39"/>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="L5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
       <c r="I6" s="39"/>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="L6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
       <c r="F7" s="23"/>
       <c r="G7" s="36"/>
       <c r="H7" s="24"/>
       <c r="I7" s="39"/>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="L7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
       <c r="F8" s="37"/>
       <c r="G8" s="26"/>
       <c r="H8" s="27"/>
       <c r="I8" s="31" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="L8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
       <c r="F9" s="28"/>
       <c r="G9" s="29"/>
       <c r="H9" s="30"/>
       <c r="I9" s="39"/>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="L9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.3">
       <c r="I10" s="39"/>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="L10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
       <c r="F11" s="23"/>
       <c r="G11" s="36"/>
       <c r="H11" s="24"/>
       <c r="I11" s="39"/>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="L11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
       <c r="F12" s="33"/>
       <c r="G12" s="26"/>
       <c r="H12" s="38"/>
       <c r="I12" s="31" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="L12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
       <c r="F13" s="28"/>
       <c r="G13" s="29"/>
       <c r="H13" s="35"/>
       <c r="I13" s="39"/>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="L13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
       <c r="I14" s="39"/>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="L14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
       <c r="F15" s="41"/>
       <c r="G15" s="32"/>
       <c r="H15" s="40"/>
       <c r="I15" s="39"/>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.3">
       <c r="F16" s="33"/>
       <c r="G16" s="26"/>
       <c r="H16" s="38"/>
@@ -1220,15 +1351,16 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:Q11"/>
+  <dimension ref="B1:Q13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="E1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1258,7 +1390,7 @@
         <v>18</v>
       </c>
       <c r="J3" s="19" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K3" s="20">
         <v>0</v>
@@ -1287,7 +1419,7 @@
         <v>19</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J4" s="22"/>
       <c r="K4" s="16" t="s">
@@ -1567,6 +1699,11 @@
       <c r="Q11" s="9">
         <f t="shared" si="1"/>
         <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="J13" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added more predicates, comments, reorganised
Added predictes for:
Generating treasures.
Assigning positions to the players
Making maze moves for the 13 combinations.
</commit_message>
<xml_diff>
--- a/Labyrinth/Labyrith_doc.xlsx
+++ b/Labyrinth/Labyrith_doc.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9840" yWindow="0" windowWidth="28800" windowHeight="13020"/>
+    <workbookView minimized="1" xWindow="11010" yWindow="0" windowWidth="18960" windowHeight="13020" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Pieces" sheetId="1" r:id="rId1"/>
@@ -1028,19 +1028,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="2.88671875" customWidth="1"/>
-    <col min="7" max="7" width="2.77734375" customWidth="1"/>
-    <col min="8" max="8" width="2.88671875" customWidth="1"/>
-    <col min="12" max="12" width="12.21875" customWidth="1"/>
+    <col min="6" max="6" width="2.85546875" customWidth="1"/>
+    <col min="7" max="7" width="2.7109375" customWidth="1"/>
+    <col min="8" max="8" width="2.85546875" customWidth="1"/>
+    <col min="12" max="12" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1060,7 +1060,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -1072,7 +1072,7 @@
       </c>
       <c r="I2" s="39"/>
     </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>2</v>
       </c>
@@ -1090,7 +1090,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -1110,7 +1110,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="F5" s="28"/>
       <c r="G5" s="34"/>
       <c r="H5" s="35"/>
@@ -1119,13 +1119,13 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="I6" s="39"/>
       <c r="L6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="F7" s="23"/>
       <c r="G7" s="36"/>
       <c r="H7" s="24"/>
@@ -1134,7 +1134,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="F8" s="37"/>
       <c r="G8" s="26"/>
       <c r="H8" s="27"/>
@@ -1145,7 +1145,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="F9" s="28"/>
       <c r="G9" s="29"/>
       <c r="H9" s="30"/>
@@ -1154,13 +1154,13 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="I10" s="39"/>
       <c r="L10" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="F11" s="23"/>
       <c r="G11" s="36"/>
       <c r="H11" s="24"/>
@@ -1169,7 +1169,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="F12" s="33"/>
       <c r="G12" s="26"/>
       <c r="H12" s="38"/>
@@ -1180,7 +1180,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="F13" s="28"/>
       <c r="G13" s="29"/>
       <c r="H13" s="35"/>
@@ -1189,19 +1189,19 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
       <c r="I14" s="39"/>
       <c r="L14" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="F15" s="41"/>
       <c r="G15" s="32"/>
       <c r="H15" s="40"/>
       <c r="I15" s="39"/>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="F16" s="33"/>
       <c r="G16" s="26"/>
       <c r="H16" s="38"/>
@@ -1209,21 +1209,21 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="17" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F17" s="42"/>
       <c r="G17" s="34"/>
       <c r="H17" s="35"/>
       <c r="I17" s="39"/>
     </row>
-    <row r="18" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="6:9" x14ac:dyDescent="0.25">
       <c r="I18" s="39"/>
     </row>
-    <row r="19" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F19" s="41"/>
       <c r="G19" s="32"/>
       <c r="H19" s="40"/>
     </row>
-    <row r="20" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F20" s="37"/>
       <c r="G20" s="26"/>
       <c r="H20" s="38"/>
@@ -1231,17 +1231,17 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="21" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F21" s="42"/>
       <c r="G21" s="29"/>
       <c r="H21" s="35"/>
     </row>
-    <row r="23" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F23" s="41"/>
       <c r="G23" s="36"/>
       <c r="H23" s="40"/>
     </row>
-    <row r="24" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F24" s="33"/>
       <c r="G24" s="26"/>
       <c r="H24" s="27"/>
@@ -1249,17 +1249,17 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F25" s="42"/>
       <c r="G25" s="34"/>
       <c r="H25" s="35"/>
     </row>
-    <row r="27" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F27" s="23"/>
       <c r="G27" s="32"/>
       <c r="H27" s="24"/>
     </row>
-    <row r="28" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F28" s="33"/>
       <c r="G28" s="26"/>
       <c r="H28" s="27"/>
@@ -1267,17 +1267,17 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="29" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F29" s="42"/>
       <c r="G29" s="34"/>
       <c r="H29" s="35"/>
     </row>
-    <row r="31" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F31" s="23"/>
       <c r="G31" s="32"/>
       <c r="H31" s="24"/>
     </row>
-    <row r="32" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F32" s="37"/>
       <c r="G32" s="26"/>
       <c r="H32" s="27"/>
@@ -1285,17 +1285,17 @@
         <v>1110</v>
       </c>
     </row>
-    <row r="33" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F33" s="28"/>
       <c r="G33" s="29"/>
       <c r="H33" s="30"/>
     </row>
-    <row r="35" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F35" s="23"/>
       <c r="G35" s="36"/>
       <c r="H35" s="24"/>
     </row>
-    <row r="36" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F36" s="33"/>
       <c r="G36" s="26"/>
       <c r="H36" s="27"/>
@@ -1303,17 +1303,17 @@
         <v>27</v>
       </c>
     </row>
-    <row r="37" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F37" s="28"/>
       <c r="G37" s="29"/>
       <c r="H37" s="35"/>
     </row>
-    <row r="39" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F39" s="41"/>
       <c r="G39" s="32"/>
       <c r="H39" s="40"/>
     </row>
-    <row r="40" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F40" s="33"/>
       <c r="G40" s="26"/>
       <c r="H40" s="27"/>
@@ -1321,19 +1321,19 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="41" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F41" s="42"/>
       <c r="G41" s="34"/>
       <c r="H41" s="35"/>
     </row>
-    <row r="43" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F43" s="23"/>
       <c r="G43" s="36">
         <v>1</v>
       </c>
       <c r="H43" s="24"/>
     </row>
-    <row r="44" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F44" s="25">
         <v>4</v>
       </c>
@@ -1342,7 +1342,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F45" s="28"/>
       <c r="G45" s="34">
         <v>3</v>
@@ -1359,20 +1359,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Q13"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="34.33203125" customWidth="1"/>
-    <col min="8" max="8" width="8.6640625" customWidth="1"/>
-    <col min="9" max="9" width="2.21875" customWidth="1"/>
-    <col min="10" max="17" width="2.6640625" customWidth="1"/>
-    <col min="18" max="18" width="2.44140625" customWidth="1"/>
+    <col min="2" max="2" width="34.28515625" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" customWidth="1"/>
+    <col min="9" max="9" width="2.28515625" customWidth="1"/>
+    <col min="10" max="17" width="2.7109375" customWidth="1"/>
+    <col min="18" max="18" width="2.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>16</v>
       </c>
@@ -1380,12 +1380,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>18</v>
       </c>
@@ -1414,7 +1414,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>19</v>
       </c>
@@ -1444,7 +1444,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>20</v>
       </c>
@@ -1476,7 +1476,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>21</v>
       </c>
@@ -1515,7 +1515,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>22</v>
       </c>
@@ -1554,7 +1554,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>23</v>
       </c>
@@ -1593,7 +1593,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
       <c r="I9" s="14">
         <v>4</v>
       </c>
@@ -1629,7 +1629,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
       <c r="I10" s="14">
         <v>5</v>
       </c>
@@ -1665,7 +1665,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I11" s="15">
         <v>6</v>
       </c>
@@ -1701,7 +1701,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
       <c r="J13" t="s">
         <v>28</v>
       </c>

</xml_diff>